<commit_message>
Two new templates - Version 2.10 and 2.11 Unlimited Flexible Monthly Template becomes Unlimited Flexible Monthly - Different Model and Unlimited Flexible Monthly - Same Model
</commit_message>
<xml_diff>
--- a/templates/VLaggregated_monthly.xlsx
+++ b/templates/VLaggregated_monthly.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="10500" windowHeight="7944"/>
+    <workbookView xWindow="285" yWindow="30" windowWidth="10500" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="VLmonthly" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>month</t>
   </si>
@@ -33,9 +33,6 @@
     <t>County</t>
   </si>
   <si>
-    <t>South-Sudan</t>
-  </si>
-  <si>
     <t>Health Factility</t>
   </si>
   <si>
@@ -136,18 +133,6 @@
   </si>
   <si>
     <t>[ VL_EPI_Gender-Type Type unspecified, Gender Unknown ]</t>
-  </si>
-  <si>
-    <t>Walgak</t>
-  </si>
-  <si>
-    <t>Jonglei state</t>
-  </si>
-  <si>
-    <t>Akobo West</t>
-  </si>
-  <si>
-    <t>JUqzTP7OtRA</t>
   </si>
   <si>
     <t>ouuid</t>
@@ -215,10 +200,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,141 +509,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.35">
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>26</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>28</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" t="s">
         <v>30</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
         <v>33</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>35</v>
       </c>
-      <c r="X3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>38</v>
       </c>
-      <c r="AA3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB3" t="s">
+    </row>
+    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -670,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -679,155 +664,70 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
       <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>11</v>
       </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
       <c r="Q4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" t="s">
         <v>10</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>11</v>
       </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
       <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" t="s">
-        <v>17</v>
-      </c>
       <c r="V4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" t="s">
         <v>16</v>
       </c>
-      <c r="X4" t="s">
-        <v>17</v>
-      </c>
       <c r="Y4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA4" t="s">
         <v>16</v>
       </c>
-      <c r="AA4" t="s">
-        <v>17</v>
-      </c>
       <c r="AB4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5">
-        <v>2015</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>53</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>53</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>35</v>
-      </c>
-      <c r="AA5">
-        <v>28</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="5" spans="1:28" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="T2:V2"/>
@@ -851,7 +751,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -863,7 +763,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Two new templates - Version 2.10 and 2.11 Unlimited Flexible Monthly Template becomes Unlimited Flexible Monthly - Different Model and Unlimited Flexible Monthly - Same Model (removed release file)
</commit_message>
<xml_diff>
--- a/templates/VLaggregated_monthly.xlsx
+++ b/templates/VLaggregated_monthly.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="10500" windowHeight="7944"/>
+    <workbookView xWindow="285" yWindow="30" windowWidth="10500" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="VLmonthly" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>month</t>
   </si>
@@ -33,9 +33,6 @@
     <t>County</t>
   </si>
   <si>
-    <t>South-Sudan</t>
-  </si>
-  <si>
     <t>Health Factility</t>
   </si>
   <si>
@@ -136,18 +133,6 @@
   </si>
   <si>
     <t>[ VL_EPI_Gender-Type Type unspecified, Gender Unknown ]</t>
-  </si>
-  <si>
-    <t>Walgak</t>
-  </si>
-  <si>
-    <t>Jonglei state</t>
-  </si>
-  <si>
-    <t>Akobo West</t>
-  </si>
-  <si>
-    <t>JUqzTP7OtRA</t>
   </si>
   <si>
     <t>ouuid</t>
@@ -215,10 +200,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,141 +509,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.35">
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>26</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>28</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>29</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" t="s">
         <v>30</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
         <v>33</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>35</v>
       </c>
-      <c r="X3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>38</v>
       </c>
-      <c r="AA3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB3" t="s">
+    </row>
+    <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -670,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -679,155 +664,70 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
       <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>11</v>
       </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
       <c r="Q4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" t="s">
         <v>10</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>11</v>
       </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
       <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" t="s">
-        <v>17</v>
-      </c>
       <c r="V4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" t="s">
         <v>16</v>
       </c>
-      <c r="X4" t="s">
-        <v>17</v>
-      </c>
       <c r="Y4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA4" t="s">
         <v>16</v>
       </c>
-      <c r="AA4" t="s">
-        <v>17</v>
-      </c>
       <c r="AB4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5">
-        <v>2015</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>53</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>53</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>35</v>
-      </c>
-      <c r="AA5">
-        <v>28</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="5" spans="1:28" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="T2:V2"/>
@@ -851,7 +751,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -863,7 +763,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>